<commit_message>
Add description to all cards
</commit_message>
<xml_diff>
--- a/Docs/Description.xlsx
+++ b/Docs/Description.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Uni\5 Semester\Praktikum\rocards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Unreal\DungeonCards\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -299,12 +299,6 @@
     <t>Restore 3 health to all minions</t>
   </si>
   <si>
-    <t>Deal 3 damage to two random enemy minions</t>
-  </si>
-  <si>
-    <t>Deal 4 damage to a minion and the enemy</t>
-  </si>
-  <si>
     <t>Give your minions stealth until your next turn</t>
   </si>
   <si>
@@ -314,9 +308,6 @@
     <t>Gain 1 mana crystal this turn only</t>
   </si>
   <si>
-    <t>Deals 2-7 damage</t>
-  </si>
-  <si>
     <t>Give a minion +2/+2 and stun it</t>
   </si>
   <si>
@@ -356,18 +347,12 @@
     <t>Deal 5 damage and summon a random minion</t>
   </si>
   <si>
-    <t>Deal 8 damage to the minion</t>
-  </si>
-  <si>
     <t>Deal 4 damage to a random enemy minion</t>
   </si>
   <si>
     <t>Spend all your mana. Restore twice that much health</t>
   </si>
   <si>
-    <t>Shoot three missiles at random enemies that deal 3 damage each.</t>
-  </si>
-  <si>
     <t>Deal 3 damage. Draw a card.</t>
   </si>
   <si>
@@ -383,9 +368,6 @@
     <t>Change a minion's attack to be equal to its health</t>
   </si>
   <si>
-    <t>Deal 1 damage to a minion and give it +2 attack</t>
-  </si>
-  <si>
     <t>Resurrect 2 different friendly minions</t>
   </si>
   <si>
@@ -407,9 +389,6 @@
     <t>Transform a minion into a poring</t>
   </si>
   <si>
-    <t>Choos a minion. Whenever it attacks, restore 4 health to your hero</t>
-  </si>
-  <si>
     <t>Shuffle all minions into your opponent's deck</t>
   </si>
   <si>
@@ -437,12 +416,6 @@
     <t>Add a random minion to your hand. It costs 2 mana less</t>
   </si>
   <si>
-    <t>Force your opponent to change a card with you.</t>
-  </si>
-  <si>
-    <t>Draw a card from your opponent's class</t>
-  </si>
-  <si>
     <t>Make 12 damage to random minions</t>
   </si>
   <si>
@@ -453,6 +426,33 @@
   </si>
   <si>
     <t>Destroy a minion and two of your mana crystals</t>
+  </si>
+  <si>
+    <t>Deal 4 damage to two random enemy minions</t>
+  </si>
+  <si>
+    <t>Deal 5 damage to a minion and the enemy</t>
+  </si>
+  <si>
+    <t>Deals 3-10 damage</t>
+  </si>
+  <si>
+    <t>Deal 10 damage to the minion</t>
+  </si>
+  <si>
+    <t>Shoot three missiles at random enemies that deal 4 damage each.</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to a minion and give it +3 attack</t>
+  </si>
+  <si>
+    <t>Choose a minion. Whenever it attacks, restore 4 health to your hero</t>
+  </si>
+  <si>
+    <t>Force your opponent to change a spell card with you.</t>
+  </si>
+  <si>
+    <t>Open 3 cards from your opponent's hand</t>
   </si>
 </sst>
 </file>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1557,7 @@
         <v>5</v>
       </c>
       <c r="I45" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -1596,7 +1596,7 @@
         <v>40</v>
       </c>
       <c r="D48">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I48" t="s">
         <v>72</v>
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -1705,7 +1705,7 @@
         <v>5</v>
       </c>
       <c r="I56" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -1747,7 +1747,7 @@
         <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
@@ -1845,7 +1845,7 @@
         <v>7</v>
       </c>
       <c r="I66" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -1855,6 +1855,9 @@
       <c r="C67" t="s">
         <v>40</v>
       </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
       <c r="I67" t="s">
         <v>87</v>
       </c>
@@ -1866,6 +1869,9 @@
       <c r="C68" t="s">
         <v>42</v>
       </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
       <c r="I68" t="s">
         <v>88</v>
       </c>
@@ -1877,6 +1883,9 @@
       <c r="C69" t="s">
         <v>44</v>
       </c>
+      <c r="D69">
+        <v>4</v>
+      </c>
       <c r="I69" t="s">
         <v>89</v>
       </c>
@@ -1888,6 +1897,9 @@
       <c r="C70" t="s">
         <v>42</v>
       </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
       <c r="I70" t="s">
         <v>90</v>
       </c>
@@ -1899,8 +1911,11 @@
       <c r="C71" t="s">
         <v>44</v>
       </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
       <c r="I71" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -1910,8 +1925,11 @@
       <c r="C72" t="s">
         <v>40</v>
       </c>
+      <c r="D72">
+        <v>4</v>
+      </c>
       <c r="I72" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -1921,8 +1939,11 @@
       <c r="C73" t="s">
         <v>42</v>
       </c>
+      <c r="D73">
+        <v>7</v>
+      </c>
       <c r="I73" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -1932,8 +1953,11 @@
       <c r="C74" t="s">
         <v>40</v>
       </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
       <c r="I74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -1943,8 +1967,11 @@
       <c r="C75" t="s">
         <v>40</v>
       </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
       <c r="I75" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -1954,8 +1981,11 @@
       <c r="C76" t="s">
         <v>40</v>
       </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
       <c r="I76" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -1965,8 +1995,11 @@
       <c r="C77" t="s">
         <v>40</v>
       </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
       <c r="I77" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -1976,8 +2009,11 @@
       <c r="C78" t="s">
         <v>42</v>
       </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
       <c r="I78" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -1987,8 +2023,11 @@
       <c r="C79" t="s">
         <v>40</v>
       </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
       <c r="I79" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -1998,8 +2037,11 @@
       <c r="C80" t="s">
         <v>40</v>
       </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
       <c r="I80" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -2009,8 +2051,11 @@
       <c r="C81" t="s">
         <v>40</v>
       </c>
+      <c r="D81">
+        <v>7</v>
+      </c>
       <c r="I81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -2020,8 +2065,11 @@
       <c r="C82" t="s">
         <v>42</v>
       </c>
+      <c r="D82">
+        <v>9</v>
+      </c>
       <c r="I82" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -2031,8 +2079,11 @@
       <c r="C83" t="s">
         <v>42</v>
       </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
       <c r="I83" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -2042,8 +2093,11 @@
       <c r="C84" t="s">
         <v>42</v>
       </c>
+      <c r="D84">
+        <v>5</v>
+      </c>
       <c r="I84" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -2053,8 +2107,11 @@
       <c r="C85" t="s">
         <v>40</v>
       </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
       <c r="I85" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -2064,8 +2121,11 @@
       <c r="C86" t="s">
         <v>40</v>
       </c>
+      <c r="D86">
+        <v>6</v>
+      </c>
       <c r="I86" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -2075,8 +2135,11 @@
       <c r="C87" t="s">
         <v>40</v>
       </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
       <c r="I87" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -2084,10 +2147,13 @@
         <v>4596</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
       </c>
       <c r="I88" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -2097,8 +2163,11 @@
       <c r="C89" t="s">
         <v>42</v>
       </c>
+      <c r="D89">
+        <v>6</v>
+      </c>
       <c r="I89" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -2108,8 +2177,11 @@
       <c r="C90" t="s">
         <v>44</v>
       </c>
+      <c r="D90">
+        <v>5</v>
+      </c>
       <c r="I90" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -2119,8 +2191,11 @@
       <c r="C91" t="s">
         <v>44</v>
       </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
       <c r="I91" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -2130,8 +2205,11 @@
       <c r="C92" t="s">
         <v>40</v>
       </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
       <c r="I92" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -2141,8 +2219,11 @@
       <c r="C93" t="s">
         <v>40</v>
       </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
       <c r="I93" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -2152,8 +2233,11 @@
       <c r="C94" t="s">
         <v>40</v>
       </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
       <c r="I94" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -2163,8 +2247,11 @@
       <c r="C95" t="s">
         <v>40</v>
       </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
       <c r="I95" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -2174,8 +2261,11 @@
       <c r="C96" t="s">
         <v>40</v>
       </c>
+      <c r="D96">
+        <v>5</v>
+      </c>
       <c r="I96" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -2185,8 +2275,11 @@
       <c r="C97" t="s">
         <v>40</v>
       </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
       <c r="I97" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -2196,8 +2289,11 @@
       <c r="C98" t="s">
         <v>40</v>
       </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
       <c r="I98" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -2205,10 +2301,13 @@
         <v>4658</v>
       </c>
       <c r="C99" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D99">
+        <v>6</v>
       </c>
       <c r="I99" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
@@ -2218,8 +2317,11 @@
       <c r="C100" t="s">
         <v>40</v>
       </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
       <c r="I100" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -2227,10 +2329,13 @@
         <v>4665</v>
       </c>
       <c r="C101" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="D101">
+        <v>6</v>
       </c>
       <c r="I101" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
@@ -2240,8 +2345,11 @@
       <c r="C102" t="s">
         <v>42</v>
       </c>
+      <c r="D102">
+        <v>3</v>
+      </c>
       <c r="I102" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -2251,8 +2359,11 @@
       <c r="C103" t="s">
         <v>40</v>
       </c>
+      <c r="D103">
+        <v>7</v>
+      </c>
       <c r="I103" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
@@ -2262,8 +2373,11 @@
       <c r="C104" t="s">
         <v>44</v>
       </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
       <c r="I104" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
@@ -2273,8 +2387,11 @@
       <c r="C105" t="s">
         <v>44</v>
       </c>
+      <c r="D105">
+        <v>5</v>
+      </c>
       <c r="I105" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
@@ -2284,8 +2401,11 @@
       <c r="C106" t="s">
         <v>40</v>
       </c>
+      <c r="D106">
+        <v>4</v>
+      </c>
       <c r="I106" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
@@ -2295,8 +2415,11 @@
       <c r="C107" t="s">
         <v>44</v>
       </c>
+      <c r="D107">
+        <v>10</v>
+      </c>
       <c r="I107" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
@@ -2306,8 +2429,11 @@
       <c r="C108" t="s">
         <v>42</v>
       </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
       <c r="I108" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -2315,10 +2441,13 @@
         <v>27110</v>
       </c>
       <c r="C109" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
       </c>
       <c r="I109" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
@@ -2328,8 +2457,11 @@
       <c r="C110" t="s">
         <v>44</v>
       </c>
+      <c r="D110">
+        <v>5</v>
+      </c>
       <c r="I110" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
@@ -2339,8 +2471,11 @@
       <c r="C111" t="s">
         <v>44</v>
       </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
       <c r="I111" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
@@ -2350,8 +2485,11 @@
       <c r="C112" t="s">
         <v>44</v>
       </c>
+      <c r="D112">
+        <v>8</v>
+      </c>
       <c r="I112" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
@@ -2361,8 +2499,11 @@
       <c r="C113" t="s">
         <v>40</v>
       </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
       <c r="I113" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
@@ -2372,8 +2513,11 @@
       <c r="C114" t="s">
         <v>40</v>
       </c>
+      <c r="D114">
+        <v>5</v>
+      </c>
       <c r="I114" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
@@ -2383,8 +2527,11 @@
       <c r="C115" t="s">
         <v>42</v>
       </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
       <c r="I115" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
@@ -2394,8 +2541,11 @@
       <c r="C116" t="s">
         <v>40</v>
       </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
       <c r="I116" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
@@ -2406,7 +2556,7 @@
         <v>40</v>
       </c>
       <c r="I117" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>